<commit_message>
shir , 32, 22, 13 - add new custumer to membership club
</commit_message>
<xml_diff>
--- a/workOnExcel/membership.xlsx
+++ b/workOnExcel/membership.xlsx
@@ -1,54 +1,57 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{125D49DC-BF60-45C5-A388-6C3F46EE0205}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="membership" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+  <si>
+    <t>first name</t>
+  </si>
+  <si>
+    <t>last name</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>adress</t>
+  </si>
+  <si>
+    <t>birthday</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
   <si>
     <t>michal</t>
   </si>
   <si>
-    <t>last name</t>
-  </si>
-  <si>
-    <t>first name</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>adress</t>
-  </si>
-  <si>
-    <t>birthday</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
     <t>tshobruzki</t>
   </si>
   <si>
+    <t>123321123</t>
+  </si>
+  <si>
     <t>bash</t>
   </si>
   <si>
+    <t>19/04/1995</t>
+  </si>
+  <si>
+    <t>0525442914</t>
+  </si>
+  <si>
     <t>shir</t>
   </si>
   <si>
@@ -58,7 +61,7 @@
     <t>dimona</t>
   </si>
   <si>
-    <t>0525442914</t>
+    <t>16/01/1995</t>
   </si>
   <si>
     <t>0502632233</t>
@@ -76,30 +79,57 @@
     <t>ashkelon</t>
   </si>
   <si>
-    <t>16/01/1995</t>
-  </si>
-  <si>
     <t>28/02/1995</t>
   </si>
   <si>
-    <t>19/04/1995</t>
-  </si>
-  <si>
     <t>0527727489</t>
   </si>
   <si>
-    <t>123321123</t>
+    <t xml:space="preserve"> igor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> feldman</t>
+  </si>
+  <si>
+    <t>242532654</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> meir grossman 5</t>
+  </si>
+  <si>
+    <t>20.09.89</t>
+  </si>
+  <si>
+    <t>0506248855</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tair</t>
+  </si>
+  <si>
+    <t>hadad</t>
+  </si>
+  <si>
+    <t>21235263</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lolo 13</t>
+  </si>
+  <si>
+    <t>14.02.77</t>
+  </si>
+  <si>
+    <t>052696322</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -124,28 +154,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -187,7 +208,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -219,27 +240,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -271,24 +274,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -464,165 +449,134 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.8984375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>234432234</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1">
-        <v>234432234</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
shir, user stories number 23, 13 : remove costumer from membrship club
</commit_message>
<xml_diff>
--- a/workOnExcel/membership.xlsx
+++ b/workOnExcel/membership.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>first name</t>
   </si>
@@ -101,24 +101,6 @@
   </si>
   <si>
     <t>0506248855</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> tair</t>
-  </si>
-  <si>
-    <t>hadad</t>
-  </si>
-  <si>
-    <t>21235263</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> lolo 13</t>
-  </si>
-  <si>
-    <t>14.02.77</t>
-  </si>
-  <si>
-    <t>052696322</t>
   </si>
 </sst>
 </file>
@@ -450,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -556,26 +538,6 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" t="s">
-        <v>34</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>